<commit_message>
adds preliminary processor scaling data to spreadsheet
</commit_message>
<xml_diff>
--- a/results/spreadsheet.xlsx
+++ b/results/spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="677" activeTab="3"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="677" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="processor scaling chart" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="symetric sheet" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="processor_scaling" localSheetId="4">'processor scaling sheet'!$A$2:$B$11</definedName>
     <definedName name="strong_scaling" localSheetId="4">'processor scaling sheet'!$A$2:$B$14</definedName>
     <definedName name="symetric" localSheetId="6">'symetric sheet'!$A$1:$B$7</definedName>
     <definedName name="thread_scaling" localSheetId="5">'thread scaling sheet'!$A$1:$B$13</definedName>
@@ -31,24 +32,32 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="strong_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling.txt">
+  <connection id="1" name="processor_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:processor_scaling.txt">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="symetric.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:symetric.txt">
+  <connection id="2" name="strong_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling.txt">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="thread_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:thread_scaling.txt">
+  <connection id="3" name="symetric.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:symetric.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="thread_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:thread_scaling.txt">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -170,47 +179,38 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'processor scaling sheet'!$A$2:$A$14</c:f>
+              <c:f>'processor scaling sheet'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>60.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -218,48 +218,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'processor scaling sheet'!$B$2:$B$14</c:f>
+              <c:f>'processor scaling sheet'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33.378</c:v>
+                  <c:v>4.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.452</c:v>
+                  <c:v>8.231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.766</c:v>
+                  <c:v>8.955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.93</c:v>
+                  <c:v>8.085</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.181</c:v>
+                  <c:v>7.721</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.691</c:v>
+                  <c:v>4.477</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.147</c:v>
+                  <c:v>13.879</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.634</c:v>
+                  <c:v>5.752</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.215</c:v>
+                  <c:v>9.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.232</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>38.56</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34.711</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>38.377</c:v>
+                  <c:v>8.906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,11 +265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2108024424"/>
-        <c:axId val="2108017192"/>
+        <c:axId val="2106417160"/>
+        <c:axId val="2106407160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2108024424"/>
+        <c:axId val="2106417160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -312,17 +303,16 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108017192"/>
+        <c:crossAx val="2106407160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2108017192"/>
+        <c:axId val="2106407160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45.0"/>
-          <c:min val="25.0"/>
+          <c:max val="20.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -360,7 +350,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108024424"/>
+        <c:crossAx val="2106417160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0"/>
@@ -426,42 +416,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.0</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>60.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -474,43 +455,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>33.378</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8904</c:v>
+                  <c:v>0.8231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9766</c:v>
+                  <c:v>0.597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.128666666666667</c:v>
+                  <c:v>0.40425</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.60905</c:v>
+                  <c:v>0.257366666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.38764</c:v>
+                  <c:v>0.111925</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.271566666666666</c:v>
+                  <c:v>0.308422222222222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.103828571428571</c:v>
+                  <c:v>0.11504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.830375</c:v>
+                  <c:v>0.178181818181818</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.760711111111111</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.7712</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.631109090909091</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.639616666666667</c:v>
+                  <c:v>0.148433333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,11 +497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109600808"/>
-        <c:axId val="2109606584"/>
+        <c:axId val="2106432104"/>
+        <c:axId val="2105714024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109600808"/>
+        <c:axId val="2106432104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,13 +535,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109606584"/>
+        <c:crossAx val="2105714024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109606584"/>
+        <c:axId val="2105714024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +575,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109600808"/>
+        <c:crossAx val="2106432104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -645,7 +617,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -763,11 +734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2118816184"/>
-        <c:axId val="2119004312"/>
+        <c:axId val="2063846648"/>
+        <c:axId val="2109560760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2118816184"/>
+        <c:axId val="2063846648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,20 +765,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119004312"/>
+        <c:crossAx val="2109560760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="40.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2119004312"/>
+        <c:axId val="2109560760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45.0"/>
@@ -836,14 +806,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118816184"/>
+        <c:crossAx val="2063846648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0"/>
@@ -851,7 +820,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -978,11 +946,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120237048"/>
-        <c:axId val="2120231816"/>
+        <c:axId val="2109450392"/>
+        <c:axId val="2118913640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120237048"/>
+        <c:axId val="2109450392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,12 +984,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120231816"/>
+        <c:crossAx val="2118913640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2120231816"/>
+        <c:axId val="2118913640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45.0"/>
@@ -1057,7 +1025,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120237048"/>
+        <c:crossAx val="2109450392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0"/>
@@ -1085,7 +1053,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1107,7 +1075,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1223,15 +1191,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="processor_scaling" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="thread_scaling" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="symetric" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="thread_scaling" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="symetric" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1556,16 +1528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1581,158 +1555,122 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>33.378</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="C2">
         <f>B2/A2</f>
-        <v>33.378</v>
+        <v>0.83000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>34.451999999999998</v>
+        <v>8.2309999999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C14" si="0">B3/A3</f>
-        <v>6.8903999999999996</v>
+        <f t="shared" ref="C3:C11" si="0">B3/A3</f>
+        <v>0.82309999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>29.765999999999998</v>
+        <v>8.9550000000000001</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>2.9765999999999999</v>
+        <v>0.59699999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>31.93</v>
+        <v>8.0850000000000009</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>2.1286666666666667</v>
+        <v>0.40425000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>32.180999999999997</v>
+        <v>7.7210000000000001</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1.6090499999999999</v>
+        <v>0.25736666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>34.691000000000003</v>
+        <v>4.4770000000000003</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.3876400000000002</v>
+        <v>0.11192500000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B8">
-        <v>38.146999999999998</v>
+        <v>13.879</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.2715666666666665</v>
+        <v>0.30842222222222221</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>38.634</v>
+        <v>5.7519999999999998</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.1038285714285714</v>
+        <v>0.11503999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B10">
-        <v>33.215000000000003</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.83037500000000009</v>
+        <v>0.17818181818181819</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B11">
-        <v>34.231999999999999</v>
+        <v>8.9060000000000006</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.76071111111111112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>38.56</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>0.7712</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <v>34.710999999999999</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>0.63110909090909084</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>60</v>
-      </c>
-      <c r="B14">
-        <v>38.377000000000002</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.63961666666666672</v>
+        <v>0.14843333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates spreadsheet with final results and figures
</commit_message>
<xml_diff>
--- a/results/spreadsheet.xlsx
+++ b/results/spreadsheet.xlsx
@@ -4,22 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="677" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="813" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="processor scaling chart" sheetId="2" r:id="rId1"/>
     <sheet name="per processor chart" sheetId="3" r:id="rId2"/>
-    <sheet name="thread scaling chart" sheetId="5" r:id="rId3"/>
-    <sheet name="symetric chart" sheetId="7" r:id="rId4"/>
-    <sheet name="processor scaling sheet" sheetId="1" r:id="rId5"/>
-    <sheet name="thread scaling sheet" sheetId="4" r:id="rId6"/>
-    <sheet name="symetric sheet" sheetId="6" r:id="rId7"/>
+    <sheet name="processor scaling sheet" sheetId="1" r:id="rId3"/>
+    <sheet name="mpi instances" sheetId="12" r:id="rId4"/>
+    <sheet name="processor count" sheetId="13" r:id="rId5"/>
+    <sheet name="per processor performance" sheetId="14" r:id="rId6"/>
+    <sheet name="Strong 4th" sheetId="8" r:id="rId7"/>
+    <sheet name="Strong 8th" sheetId="9" r:id="rId8"/>
+    <sheet name="Strong 16th" sheetId="10" r:id="rId9"/>
+    <sheet name="Strong 32th" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="processor_scaling" localSheetId="4">'processor scaling sheet'!$A$2:$B$11</definedName>
-    <definedName name="strong_scaling" localSheetId="4">'processor scaling sheet'!$A$2:$B$14</definedName>
-    <definedName name="symetric" localSheetId="6">'symetric sheet'!$A$1:$B$7</definedName>
-    <definedName name="thread_scaling" localSheetId="5">'thread scaling sheet'!$A$1:$B$13</definedName>
+    <definedName name="processor_scaling" localSheetId="2">'processor scaling sheet'!$A$2:$B$11</definedName>
+    <definedName name="strong_scaling" localSheetId="2">'processor scaling sheet'!$A$2:$B$14</definedName>
+    <definedName name="strong_scaling_16_results" localSheetId="8">'Strong 16th'!$A$2:$D$8</definedName>
+    <definedName name="strong_scaling_32_results" localSheetId="9">'Strong 32th'!$A$2:$D$8</definedName>
+    <definedName name="strong_scaling_4_results" localSheetId="6">'Strong 4th'!$A$2:$D$12</definedName>
+    <definedName name="strong_scaling_8_results" localSheetId="7">'Strong 8th'!$A$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="140000" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +45,39 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="strong_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="strong_scaling_16_results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling_16_results.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="strong_scaling_32_results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling_32_results.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="strong_scaling_4_results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling_4_results.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="strong_scaling_8_results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling_8_results.txt">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="strong_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:strong_scaling.txt">
       <textFields count="2">
         <textField/>
@@ -48,7 +85,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="symetric.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="symetric.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:symetric.txt">
       <textFields count="2">
         <textField/>
@@ -56,7 +93,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="thread_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="thread_scaling.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:andrewadams:Desktop:parallel_final:results:thread_scaling.txt">
       <textFields count="2">
         <textField/>
@@ -68,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>number of processors</t>
   </si>
@@ -78,15 +115,50 @@
   <si>
     <t>ns/day per processor</t>
   </si>
+  <si>
+    <t>mpi instances</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>processor count</t>
+  </si>
+  <si>
+    <t>performance/processor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,13 +181,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -265,11 +354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2106417160"/>
-        <c:axId val="2106407160"/>
+        <c:axId val="2073909048"/>
+        <c:axId val="2073916216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2106417160"/>
+        <c:axId val="2073909048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,13 +392,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106407160"/>
+        <c:crossAx val="2073916216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2106407160"/>
+        <c:axId val="2073916216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -350,7 +439,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106417160"/>
+        <c:crossAx val="2073909048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0"/>
@@ -497,11 +586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2106432104"/>
-        <c:axId val="2105714024"/>
+        <c:axId val="2074352424"/>
+        <c:axId val="2074285704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2106432104"/>
+        <c:axId val="2074352424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,13 +624,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105714024"/>
+        <c:crossAx val="2074285704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="5.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2105714024"/>
+        <c:axId val="2074285704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +664,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106432104"/>
+        <c:crossAx val="2074352424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -612,11 +701,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Thread Scaling</a:t>
+              <a:t>Performance</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. MPI Instances</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -628,98 +723,287 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>4 thread</c:v>
+          </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'thread scaling sheet'!$A$1:$A$13</c:f>
+              <c:f>'Strong 4th'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>40.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>140.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>160.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>180.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>220.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>240.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'thread scaling sheet'!$B$1:$B$13</c:f>
+              <c:f>'Strong 4th'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>32.184</c:v>
+                  <c:v>1.164</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.309</c:v>
+                  <c:v>4.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.641</c:v>
+                  <c:v>8.231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.643</c:v>
+                  <c:v>8.955</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.242</c:v>
+                  <c:v>8.085</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.581</c:v>
+                  <c:v>7.721</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.503</c:v>
+                  <c:v>4.477</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.629</c:v>
+                  <c:v>3.879</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.948</c:v>
+                  <c:v>5.752</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.305</c:v>
+                  <c:v>9.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.082</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>35.008</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>33.837</c:v>
+                  <c:v>8.906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>8 thread</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.642</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>16 thread</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.181</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.483</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.723</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>32 thread</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.239</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.041</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.937</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,11 +1018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2063846648"/>
-        <c:axId val="2109560760"/>
+        <c:axId val="2116935400"/>
+        <c:axId val="2116938424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2063846648"/>
+        <c:axId val="2116935400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,33 +1039,31 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
+                  <a:t>MPI</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Threads</a:t>
+                  <a:t> Instances</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109560760"/>
+        <c:crossAx val="2116938424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="40.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109560760"/>
+        <c:axId val="2116938424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45.0"/>
-          <c:min val="25.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -796,30 +1078,26 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Performance</a:t>
+                  <a:t>Performance (ns/day)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ns/day)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063846648"/>
+        <c:crossAx val="2116935400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="1.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -854,11 +1132,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Symetric</a:t>
+              <a:t>Performance</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Performance</a:t>
+              <a:t> vs. Processor Utilization</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -876,12 +1154,15 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>4 threads</c:v>
+          </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'symetric sheet'!$A$1:$A$7</c:f>
+              <c:f>'Strong 4th'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -901,6 +1182,18 @@
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>60.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -908,30 +1201,240 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'symetric sheet'!$B$1:$B$7</c:f>
+              <c:f>'Strong 4th'!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.955</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.085</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.721</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.879</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>8 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.642</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>16 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>30.927</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.515</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.798</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.936</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.722</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.738</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.51</c:v>
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.181</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.483</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.723</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>32 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.239</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.041</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.937</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.976</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -946,11 +1449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109450392"/>
-        <c:axId val="2118913640"/>
+        <c:axId val="2081454824"/>
+        <c:axId val="2118007416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109450392"/>
+        <c:axId val="2081454824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,11 +1470,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
+                  <a:t>Processors</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Processors</a:t>
+                  <a:t> Utilized by Simulation</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -981,19 +1484,17 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118913640"/>
+        <c:crossAx val="2118007416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2118913640"/>
+        <c:axId val="2118007416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45.0"/>
-          <c:min val="25.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1022,15 +1523,456 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109450392"/>
+        <c:crossAx val="2081454824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="1.0"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Per Processor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 4th'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 4th'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8231</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.257366666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.111925</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0862</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11504</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.178181818181818</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.148433333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>8 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 8th'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0880666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.073725</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0834666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>16 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 16th'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.95075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0240714285714286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0134166666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0576590909090909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0287166666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>32 threads</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Strong 32th'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.782</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3899375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.376708333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27928125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0203333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0175535714285714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2121843880"/>
+        <c:axId val="2120102200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2121843880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processors Utilized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> by Simulation</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120102200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2120102200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Performance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ns/processor day)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121843880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1053,7 +1995,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1072,6 +2014,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -1190,20 +2143,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8580438" cy="5834063"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="processor_scaling" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="thread_scaling" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling_4_results" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="symetric" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling_8_results" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling_16_results" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strong_scaling_32_results" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1685,118 +2673,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
-        <v>32.183999999999997</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>D2/B2</f>
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="D2">
+        <v>1.1639999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="0">A3</f>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="1">D3/B3</f>
+        <v>0.83000000000000007</v>
+      </c>
+      <c r="D3">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.82309999999999994</v>
+      </c>
+      <c r="D4">
+        <v>8.2309999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="D5">
+        <v>8.9550000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>34.308999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.40425000000000005</v>
+      </c>
+      <c r="D6">
+        <v>8.0850000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.25736666666666669</v>
+      </c>
+      <c r="D7">
+        <v>7.7210000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>40</v>
       </c>
-      <c r="B3">
-        <v>33.640999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.11192500000000001</v>
+      </c>
+      <c r="D8">
+        <v>4.4770000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.879</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.11503999999999999</v>
+      </c>
+      <c r="D10">
+        <v>5.7519999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.17818181818181819</v>
+      </c>
+      <c r="D11">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
         <v>60</v>
       </c>
-      <c r="B4">
-        <v>36.643000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>80</v>
-      </c>
-      <c r="B5">
-        <v>35.241999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>38.581000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>120</v>
-      </c>
-      <c r="B7">
-        <v>33.503</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>140</v>
-      </c>
-      <c r="B8">
-        <v>33.628999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>160</v>
-      </c>
-      <c r="B9">
-        <v>32.948</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>180</v>
-      </c>
-      <c r="B10">
-        <v>34.305</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>200</v>
-      </c>
-      <c r="B11">
-        <v>33.082000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>220</v>
-      </c>
       <c r="B12">
-        <v>35.008000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>240</v>
-      </c>
-      <c r="B13">
-        <v>33.837000000000003</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.14843333333333333</v>
+      </c>
+      <c r="D12">
+        <v>8.9060000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1811,70 +2889,432 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>30.927</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B2">
+        <f>A2*2</f>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>D2/B2</f>
+        <v>1.101</v>
+      </c>
+      <c r="D2">
+        <v>2.202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B7" si="0">A3*2</f>
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="1">D3/B3</f>
+        <v>0.78410000000000002</v>
+      </c>
+      <c r="D3">
+        <v>7.8410000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>8.8066666666666668E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.6419999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>7.3724999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.9489999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>8.3466666666666661E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2*4</f>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f>D2/B2</f>
+        <v>0.95074999999999998</v>
+      </c>
+      <c r="D2">
+        <v>3.8029999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B8" si="0">A3*4</f>
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="1">D3/B3</f>
+        <v>0.60825000000000007</v>
+      </c>
+      <c r="D3">
+        <v>7.2990000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>5</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>9.049999999999999E-3</v>
+      </c>
+      <c r="D4">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>2.4071428571428573E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.3416666666666667E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>5.765909090909091E-2</v>
+      </c>
+      <c r="D7">
+        <v>2.5369999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2.8716666666666668E-2</v>
+      </c>
+      <c r="D8">
+        <v>1.7230000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>31.515000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <f>A2*8</f>
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <f>D2/B2</f>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D2">
+        <v>6.2560000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>40.798000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <f t="shared" ref="B3:B9" si="0">A3*8</f>
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="1">D3/B3</f>
+        <v>0.38993749999999999</v>
+      </c>
+      <c r="D3">
+        <v>6.2389999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>35.936</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.37670833333333337</v>
+      </c>
+      <c r="D4">
+        <v>9.0410000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>39.722000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.27928124999999998</v>
+      </c>
+      <c r="D5">
+        <v>8.9369999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>37.738</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.7599999999999998E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.70399999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>38.51</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2.0333333333333332E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.7553571428571429E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.98299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>